<commit_message>
Tentativo click destro sulla mappa
</commit_message>
<xml_diff>
--- a/To do list.xlsx
+++ b/To do list.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\colav\Documents\GitHub\Tesi-di-laurea\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{60B3AC49-F027-4347-89DE-8576AC4C0AFD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5C2F1D2F-E467-40AE-B7DE-4547EFE8A93C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{374C2BF4-237C-43AC-A09E-A9E5892F3E3D}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{374C2BF4-237C-43AC-A09E-A9E5892F3E3D}"/>
   </bookViews>
   <sheets>
     <sheet name="Foglio1" sheetId="1" r:id="rId1"/>
@@ -460,18 +460,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E90CAFAD-83F7-436E-9F51-FAFD1DE9C298}">
   <dimension ref="A1:D21"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="A21" sqref="A21"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="B20" sqref="B20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="87.5703125" style="1" customWidth="1"/>
-    <col min="2" max="2" width="60.5703125" style="1" customWidth="1"/>
-    <col min="3" max="16384" width="8.85546875" style="1"/>
+    <col min="1" max="1" width="87.5546875" style="1" customWidth="1"/>
+    <col min="2" max="2" width="60.5546875" style="1" customWidth="1"/>
+    <col min="3" max="16384" width="8.88671875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -485,67 +485,67 @@
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="12" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A13" s="1" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A15" s="1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A16" s="1" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="18" spans="1:2" ht="45" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A18" s="1" t="s">
         <v>13</v>
       </c>
@@ -553,7 +553,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A19" s="1" t="s">
         <v>18</v>
       </c>
@@ -561,7 +561,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="20" spans="1:2" ht="120" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:2" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A20" s="1" t="s">
         <v>14</v>
       </c>
@@ -569,7 +569,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A21" s="1" t="s">
         <v>22</v>
       </c>

</xml_diff>

<commit_message>
Modifiche alle azioni del robot.
Ora se il robot si trova nella stessa cella dell'entità e viene richiamato il frame TAKING o MANIPULATING, il robot non si sposterà più ma afferra direttamente l'oggetto che si trova nella sua stessa cella.
</commit_message>
<xml_diff>
--- a/To do list.xlsx
+++ b/To do list.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\colav\Documents\GitHub\Tesi-di-laurea\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D1EBAEEF-6B68-4972-B730-2E4BE2FEDD30}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E88196AA-5FAC-4ADF-B574-0A6CA5741BFD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{374C2BF4-237C-43AC-A09E-A9E5892F3E3D}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="32">
   <si>
     <t>To do list progetto</t>
   </si>
@@ -100,9 +100,6 @@
     <t>Possilità tramite opzioni di personalizzare l'id (ex lettera+numero, 3 lettere + numero, nome completo + numero (table1) )</t>
   </si>
   <si>
-    <t>Click destro (https://p5js.org/reference/#/p5/mouseButton però rimuovere la tendina di default su browser) + alert conferma di rimozione cella + rimuovere entità sulla cella. Se c'è un entità più grande di una cella, rimuoverla anche dalle altre + controllo entità sopra/sotto e in caso metterlo "on the floor" facendo apparire un alert riguardo questo caso (sicuro di voler rimuovere la cella con il suo contenuto? tutti gli oggetti sopr/sotto all'entità che si trovano in questa cella veranno messi per terra)</t>
-  </si>
-  <si>
     <t>5. Spostare gli ip nel file di configurazione</t>
   </si>
   <si>
@@ -118,9 +115,6 @@
     <t>Note modifica</t>
   </si>
   <si>
-    <t>Per ora, le entità sopra sotto all'entità che occupa uno spazio maggiore di 1 verranno cancellate anche loro. Varrà poi modificato e le entità esterne alla cella cancellata verranno poggiate per terra.</t>
-  </si>
-  <si>
     <t>Se la mappa supera la grandezza della pagina web, ridimensionare le celle rendendole più piccole per farle entrare tutte.</t>
   </si>
   <si>
@@ -128,6 +122,15 @@
   </si>
   <si>
     <t>Quando viene cliccato l'agente sulla mappa non viene mostrato nella tabella delle informazioni</t>
+  </si>
+  <si>
+    <t>Click destro (https://p5js.org/reference/#/p5/mouseButton però rimuovere la tendina di default su browser) + alert conferma di rimozione cella + rimuovere entità sulla cella. Se c'è un entità più grande di una cella, rimuoverla anche dalle altre + controllo entità sopra/sotto e in caso metterlo "on the floor" facendo apparire un alert riguardo questo caso (sicuro di voler rimuovere la cella con il suo contenuto? tutti gli oggetti sopr/sotto all'entità che si trovano in questa cella veranno rimossi)</t>
+  </si>
+  <si>
+    <t>4. Problema con posizionamento degli oggetti sopra ad un altro</t>
+  </si>
+  <si>
+    <t>Rimuoverere possibilità di mettere più oggetti in una cella sopra ad un altro oggetto. (Ex. Si possono mettere più pc sopra al tavolo nella stessa cella).</t>
   </si>
 </sst>
 </file>
@@ -514,10 +517,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E90CAFAD-83F7-436E-9F51-FAFD1DE9C298}">
-  <dimension ref="A1:E22"/>
+  <dimension ref="A1:E23"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -544,7 +547,7 @@
         <v>17</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="2" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
@@ -552,7 +555,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="C2" s="4"/>
     </row>
@@ -561,7 +564,7 @@
         <v>2</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D3" s="2">
         <v>44773</v>
@@ -620,7 +623,7 @@
         <v>10</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="C13" s="4"/>
     </row>
@@ -632,7 +635,7 @@
         <v>11</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="C15" s="4"/>
     </row>
@@ -642,58 +645,69 @@
       </c>
       <c r="C16" s="4"/>
     </row>
-    <row r="17" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A17" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B17" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="B17" s="1" t="s">
-        <v>25</v>
-      </c>
       <c r="C17" s="4"/>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A18" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>31</v>
+      </c>
       <c r="C18" s="4"/>
     </row>
-    <row r="19" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A19" s="1" t="s">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="C19" s="4"/>
+    </row>
+    <row r="20" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A20" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="B19" s="1" t="s">
+      <c r="B20" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="C19" s="4"/>
-    </row>
-    <row r="20" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A20" s="1" t="s">
+      <c r="C20" s="4"/>
+    </row>
+    <row r="21" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A21" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="B20" s="1" t="s">
+      <c r="B21" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="C20" s="4"/>
-    </row>
-    <row r="21" spans="1:5" ht="115.2" x14ac:dyDescent="0.3">
-      <c r="A21" s="1" t="s">
+      <c r="C21" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="D21" s="2">
+        <v>44776</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" ht="115.2" x14ac:dyDescent="0.3">
+      <c r="A22" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="B21" s="1" t="s">
+      <c r="B22" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="C22" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="D22" s="2">
+        <v>44773</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A23" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="C21" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="D21" s="2">
-        <v>44773</v>
-      </c>
-      <c r="E21" s="1" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A22" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="C22" s="4"/>
+      <c r="C23" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Fix max righe/colonne - other
Fixato il numero massimo di righe e colonne se inserito manualmente.
Modificata estetica FE
</commit_message>
<xml_diff>
--- a/To do list.xlsx
+++ b/To do list.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\baste\Desktop\Lavoro\reveal\python_code\Interfaccia-Interazione-Uomo-Robot\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\colav\Documents\GitHub\Tesi-di-laurea\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C4458EA0-1A4F-4BFB-B04B-D85E585C301A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1CD0DAB0-2FFB-4C4C-BC4C-F8FDE0B1B141}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16896" xr2:uid="{374C2BF4-237C-43AC-A09E-A9E5892F3E3D}"/>
+    <workbookView xWindow="2340" yWindow="2340" windowWidth="21600" windowHeight="11295" xr2:uid="{374C2BF4-237C-43AC-A09E-A9E5892F3E3D}"/>
   </bookViews>
   <sheets>
     <sheet name="Foglio1" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="39">
   <si>
     <t>To do list progetto</t>
   </si>
@@ -155,6 +155,9 @@
 - aggiungere 2 pulsanti (icone: pollice in su e pollice in giù) vicino Answer che fanno una post su URL da definire
 - (IN FUTURO: fare in modo che se l'utente preme su pollice in giù, allora Answer diventa modificabile e deve scrivere lui la risposta giusta)
 - aggiungere altro pulsante che invia il feedback</t>
+  </si>
+  <si>
+    <t>Mancante: URL</t>
   </si>
 </sst>
 </file>
@@ -547,20 +550,20 @@
   <dimension ref="A1:E28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="66.77734375" style="1" customWidth="1"/>
-    <col min="2" max="2" width="60.5546875" style="1" customWidth="1"/>
-    <col min="3" max="3" width="8.88671875" style="1"/>
-    <col min="4" max="4" width="14.44140625" style="1" customWidth="1"/>
-    <col min="5" max="5" width="43.5546875" style="1" customWidth="1"/>
-    <col min="6" max="16384" width="8.88671875" style="1"/>
+    <col min="1" max="1" width="66.7109375" style="1" customWidth="1"/>
+    <col min="2" max="2" width="60.5703125" style="1" customWidth="1"/>
+    <col min="3" max="3" width="8.85546875" style="1"/>
+    <col min="4" max="4" width="14.42578125" style="1" customWidth="1"/>
+    <col min="5" max="5" width="43.5703125" style="1" customWidth="1"/>
+    <col min="6" max="16384" width="8.85546875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" s="3" customFormat="1" ht="18" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" s="3" customFormat="1" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -577,28 +580,41 @@
         <v>25</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C2" s="4"/>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>32</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="C3" s="4"/>
-    </row>
-    <row r="4" spans="1:5" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="C3" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="D3" s="2">
+        <v>44933</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" ht="60" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>34</v>
       </c>
       <c r="B4" s="5" t="s">
         <v>36</v>
       </c>
-      <c r="C4" s="4"/>
-    </row>
-    <row r="5" spans="1:5" ht="144" x14ac:dyDescent="0.3">
+      <c r="C4" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="D4" s="2">
+        <v>44933</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" ht="180" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>35</v>
       </c>
@@ -607,10 +623,10 @@
       </c>
       <c r="C5" s="4"/>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C6" s="4"/>
     </row>
-    <row r="7" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>1</v>
       </c>
@@ -619,7 +635,7 @@
       </c>
       <c r="C7" s="4"/>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>2</v>
       </c>
@@ -630,55 +646,55 @@
         <v>44773</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C9" s="4"/>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>3</v>
       </c>
       <c r="C10" s="4"/>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>4</v>
       </c>
       <c r="C11" s="4"/>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>5</v>
       </c>
       <c r="C12" s="4"/>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C13" s="4"/>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>6</v>
       </c>
       <c r="C14" s="4"/>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>7</v>
       </c>
       <c r="C15" s="4"/>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>8</v>
       </c>
       <c r="C16" s="4"/>
     </row>
-    <row r="17" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
         <v>9</v>
       </c>
       <c r="C17" s="4"/>
     </row>
-    <row r="18" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
         <v>10</v>
       </c>
@@ -687,10 +703,10 @@
       </c>
       <c r="C18" s="4"/>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C19" s="4"/>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
         <v>11</v>
       </c>
@@ -699,13 +715,13 @@
       </c>
       <c r="C20" s="4"/>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
         <v>12</v>
       </c>
       <c r="C21" s="4"/>
     </row>
-    <row r="22" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
         <v>23</v>
       </c>
@@ -714,7 +730,7 @@
       </c>
       <c r="C22" s="4"/>
     </row>
-    <row r="23" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
         <v>30</v>
       </c>
@@ -723,10 +739,10 @@
       </c>
       <c r="C23" s="4"/>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C24" s="4"/>
     </row>
-    <row r="25" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
         <v>13</v>
       </c>
@@ -735,7 +751,7 @@
       </c>
       <c r="C25" s="4"/>
     </row>
-    <row r="26" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
         <v>18</v>
       </c>
@@ -749,7 +765,7 @@
         <v>44776</v>
       </c>
     </row>
-    <row r="27" spans="1:4" ht="115.2" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:4" ht="120" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
         <v>14</v>
       </c>
@@ -763,7 +779,7 @@
         <v>44773</v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
         <v>21</v>
       </c>

</xml_diff>

<commit_message>
Revert "Fix max righe/colonne - other"
This reverts commit 58be4683e8cde7eed520989eca3c9a2ac631ab33.
</commit_message>
<xml_diff>
--- a/To do list.xlsx
+++ b/To do list.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\colav\Documents\GitHub\Tesi-di-laurea\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\baste\Desktop\Lavoro\reveal\python_code\Interfaccia-Interazione-Uomo-Robot\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1CD0DAB0-2FFB-4C4C-BC4C-F8FDE0B1B141}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C4458EA0-1A4F-4BFB-B04B-D85E585C301A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2340" yWindow="2340" windowWidth="21600" windowHeight="11295" xr2:uid="{374C2BF4-237C-43AC-A09E-A9E5892F3E3D}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16896" xr2:uid="{374C2BF4-237C-43AC-A09E-A9E5892F3E3D}"/>
   </bookViews>
   <sheets>
     <sheet name="Foglio1" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="38">
   <si>
     <t>To do list progetto</t>
   </si>
@@ -155,9 +155,6 @@
 - aggiungere 2 pulsanti (icone: pollice in su e pollice in giù) vicino Answer che fanno una post su URL da definire
 - (IN FUTURO: fare in modo che se l'utente preme su pollice in giù, allora Answer diventa modificabile e deve scrivere lui la risposta giusta)
 - aggiungere altro pulsante che invia il feedback</t>
-  </si>
-  <si>
-    <t>Mancante: URL</t>
   </si>
 </sst>
 </file>
@@ -550,20 +547,20 @@
   <dimension ref="A1:E28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="66.7109375" style="1" customWidth="1"/>
-    <col min="2" max="2" width="60.5703125" style="1" customWidth="1"/>
-    <col min="3" max="3" width="8.85546875" style="1"/>
-    <col min="4" max="4" width="14.42578125" style="1" customWidth="1"/>
-    <col min="5" max="5" width="43.5703125" style="1" customWidth="1"/>
-    <col min="6" max="16384" width="8.85546875" style="1"/>
+    <col min="1" max="1" width="66.77734375" style="1" customWidth="1"/>
+    <col min="2" max="2" width="60.5546875" style="1" customWidth="1"/>
+    <col min="3" max="3" width="8.88671875" style="1"/>
+    <col min="4" max="4" width="14.44140625" style="1" customWidth="1"/>
+    <col min="5" max="5" width="43.5546875" style="1" customWidth="1"/>
+    <col min="6" max="16384" width="8.88671875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" s="3" customFormat="1" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" s="3" customFormat="1" ht="18" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -580,41 +577,28 @@
         <v>25</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="C2" s="4"/>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>32</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="C3" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="D3" s="2">
-        <v>44933</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+      <c r="C3" s="4"/>
+    </row>
+    <row r="4" spans="1:5" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>34</v>
       </c>
       <c r="B4" s="5" t="s">
         <v>36</v>
       </c>
-      <c r="C4" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="D4" s="2">
-        <v>44933</v>
-      </c>
-      <c r="E4" s="1" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" ht="180" x14ac:dyDescent="0.25">
+      <c r="C4" s="4"/>
+    </row>
+    <row r="5" spans="1:5" ht="144" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
         <v>35</v>
       </c>
@@ -623,10 +607,10 @@
       </c>
       <c r="C5" s="4"/>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="C6" s="4"/>
     </row>
-    <row r="7" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
         <v>1</v>
       </c>
@@ -635,7 +619,7 @@
       </c>
       <c r="C7" s="4"/>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
         <v>2</v>
       </c>
@@ -646,55 +630,55 @@
         <v>44773</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
       <c r="C9" s="4"/>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
         <v>3</v>
       </c>
       <c r="C10" s="4"/>
     </row>
-    <row r="11" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
         <v>4</v>
       </c>
       <c r="C11" s="4"/>
     </row>
-    <row r="12" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
         <v>5</v>
       </c>
       <c r="C12" s="4"/>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
       <c r="C13" s="4"/>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A14" s="1" t="s">
         <v>6</v>
       </c>
       <c r="C14" s="4"/>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A15" s="1" t="s">
         <v>7</v>
       </c>
       <c r="C15" s="4"/>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A16" s="1" t="s">
         <v>8</v>
       </c>
       <c r="C16" s="4"/>
     </row>
-    <row r="17" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A17" s="1" t="s">
         <v>9</v>
       </c>
       <c r="C17" s="4"/>
     </row>
-    <row r="18" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A18" s="1" t="s">
         <v>10</v>
       </c>
@@ -703,10 +687,10 @@
       </c>
       <c r="C18" s="4"/>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
       <c r="C19" s="4"/>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A20" s="1" t="s">
         <v>11</v>
       </c>
@@ -715,13 +699,13 @@
       </c>
       <c r="C20" s="4"/>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A21" s="1" t="s">
         <v>12</v>
       </c>
       <c r="C21" s="4"/>
     </row>
-    <row r="22" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A22" s="1" t="s">
         <v>23</v>
       </c>
@@ -730,7 +714,7 @@
       </c>
       <c r="C22" s="4"/>
     </row>
-    <row r="23" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A23" s="1" t="s">
         <v>30</v>
       </c>
@@ -739,10 +723,10 @@
       </c>
       <c r="C23" s="4"/>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
       <c r="C24" s="4"/>
     </row>
-    <row r="25" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A25" s="1" t="s">
         <v>13</v>
       </c>
@@ -751,7 +735,7 @@
       </c>
       <c r="C25" s="4"/>
     </row>
-    <row r="26" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A26" s="1" t="s">
         <v>18</v>
       </c>
@@ -765,7 +749,7 @@
         <v>44776</v>
       </c>
     </row>
-    <row r="27" spans="1:4" ht="120" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:4" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A27" s="1" t="s">
         <v>14</v>
       </c>
@@ -779,7 +763,7 @@
         <v>44773</v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A28" s="1" t="s">
         <v>21</v>
       </c>

</xml_diff>

<commit_message>
Revert "Revert "Fix max righe/colonne - other""
This reverts commit eb656f9519ee3c857465ff6bc5095b2ce71469d6.
</commit_message>
<xml_diff>
--- a/To do list.xlsx
+++ b/To do list.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\baste\Desktop\Lavoro\reveal\python_code\Interfaccia-Interazione-Uomo-Robot\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\colav\Documents\GitHub\Tesi-di-laurea\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C4458EA0-1A4F-4BFB-B04B-D85E585C301A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1CD0DAB0-2FFB-4C4C-BC4C-F8FDE0B1B141}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16896" xr2:uid="{374C2BF4-237C-43AC-A09E-A9E5892F3E3D}"/>
+    <workbookView xWindow="2340" yWindow="2340" windowWidth="21600" windowHeight="11295" xr2:uid="{374C2BF4-237C-43AC-A09E-A9E5892F3E3D}"/>
   </bookViews>
   <sheets>
     <sheet name="Foglio1" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="39">
   <si>
     <t>To do list progetto</t>
   </si>
@@ -155,6 +155,9 @@
 - aggiungere 2 pulsanti (icone: pollice in su e pollice in giù) vicino Answer che fanno una post su URL da definire
 - (IN FUTURO: fare in modo che se l'utente preme su pollice in giù, allora Answer diventa modificabile e deve scrivere lui la risposta giusta)
 - aggiungere altro pulsante che invia il feedback</t>
+  </si>
+  <si>
+    <t>Mancante: URL</t>
   </si>
 </sst>
 </file>
@@ -547,20 +550,20 @@
   <dimension ref="A1:E28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="66.77734375" style="1" customWidth="1"/>
-    <col min="2" max="2" width="60.5546875" style="1" customWidth="1"/>
-    <col min="3" max="3" width="8.88671875" style="1"/>
-    <col min="4" max="4" width="14.44140625" style="1" customWidth="1"/>
-    <col min="5" max="5" width="43.5546875" style="1" customWidth="1"/>
-    <col min="6" max="16384" width="8.88671875" style="1"/>
+    <col min="1" max="1" width="66.7109375" style="1" customWidth="1"/>
+    <col min="2" max="2" width="60.5703125" style="1" customWidth="1"/>
+    <col min="3" max="3" width="8.85546875" style="1"/>
+    <col min="4" max="4" width="14.42578125" style="1" customWidth="1"/>
+    <col min="5" max="5" width="43.5703125" style="1" customWidth="1"/>
+    <col min="6" max="16384" width="8.85546875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" s="3" customFormat="1" ht="18" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" s="3" customFormat="1" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -577,28 +580,41 @@
         <v>25</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C2" s="4"/>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>32</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="C3" s="4"/>
-    </row>
-    <row r="4" spans="1:5" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="C3" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="D3" s="2">
+        <v>44933</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" ht="60" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>34</v>
       </c>
       <c r="B4" s="5" t="s">
         <v>36</v>
       </c>
-      <c r="C4" s="4"/>
-    </row>
-    <row r="5" spans="1:5" ht="144" x14ac:dyDescent="0.3">
+      <c r="C4" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="D4" s="2">
+        <v>44933</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" ht="180" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>35</v>
       </c>
@@ -607,10 +623,10 @@
       </c>
       <c r="C5" s="4"/>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C6" s="4"/>
     </row>
-    <row r="7" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>1</v>
       </c>
@@ -619,7 +635,7 @@
       </c>
       <c r="C7" s="4"/>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>2</v>
       </c>
@@ -630,55 +646,55 @@
         <v>44773</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C9" s="4"/>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>3</v>
       </c>
       <c r="C10" s="4"/>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>4</v>
       </c>
       <c r="C11" s="4"/>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>5</v>
       </c>
       <c r="C12" s="4"/>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C13" s="4"/>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>6</v>
       </c>
       <c r="C14" s="4"/>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>7</v>
       </c>
       <c r="C15" s="4"/>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>8</v>
       </c>
       <c r="C16" s="4"/>
     </row>
-    <row r="17" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
         <v>9</v>
       </c>
       <c r="C17" s="4"/>
     </row>
-    <row r="18" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
         <v>10</v>
       </c>
@@ -687,10 +703,10 @@
       </c>
       <c r="C18" s="4"/>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C19" s="4"/>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
         <v>11</v>
       </c>
@@ -699,13 +715,13 @@
       </c>
       <c r="C20" s="4"/>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
         <v>12</v>
       </c>
       <c r="C21" s="4"/>
     </row>
-    <row r="22" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
         <v>23</v>
       </c>
@@ -714,7 +730,7 @@
       </c>
       <c r="C22" s="4"/>
     </row>
-    <row r="23" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
         <v>30</v>
       </c>
@@ -723,10 +739,10 @@
       </c>
       <c r="C23" s="4"/>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C24" s="4"/>
     </row>
-    <row r="25" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
         <v>13</v>
       </c>
@@ -735,7 +751,7 @@
       </c>
       <c r="C25" s="4"/>
     </row>
-    <row r="26" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
         <v>18</v>
       </c>
@@ -749,7 +765,7 @@
         <v>44776</v>
       </c>
     </row>
-    <row r="27" spans="1:4" ht="115.2" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:4" ht="120" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
         <v>14</v>
       </c>
@@ -763,7 +779,7 @@
         <v>44773</v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
         <v>21</v>
       </c>

</xml_diff>